<commit_message>
Update code to parse different sheets
</commit_message>
<xml_diff>
--- a/products/FCN Try/input.xlsx
+++ b/products/FCN Try/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TS Generator\Template-Generator\products\FCN Try\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3121A855-F424-4A78-A9BB-D8C67D01F601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07339CDA-CD75-43E9-B121-22260AD3589C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FCCAF5-58C3-4D44-9C49-A1FEBE5D251F}">
   <dimension ref="B3:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C74DF-B7C9-47E9-9B7B-A13599351EEC}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add table creation functionality
</commit_message>
<xml_diff>
--- a/products/FCN Try/input.xlsx
+++ b/products/FCN Try/input.xlsx
@@ -8,15 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TS Generator\Template-Generator\products\FCN Try\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07339CDA-CD75-43E9-B121-22260AD3589C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54014CC7-753B-4872-9195-6AB36E0BB215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Manually" sheetId="2" r:id="rId2"/>
     <sheet name="Observation Table" sheetId="3" r:id="rId3"/>
+    <sheet name="Share Basket Table" sheetId="6" r:id="rId4"/>
+    <sheet name="BBG CODES" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="163">
   <si>
     <t>Product</t>
   </si>
@@ -149,13 +154,391 @@
   </si>
   <si>
     <t>Barrier Price Percentage (t)</t>
+  </si>
+  <si>
+    <t>BBG Code</t>
+  </si>
+  <si>
+    <t>Share Name</t>
+  </si>
+  <si>
+    <t>Exchange</t>
+  </si>
+  <si>
+    <t>GOOGL UQ</t>
+  </si>
+  <si>
+    <t>Alphabet Inc.</t>
+  </si>
+  <si>
+    <t>NASDAQ Global Select Market</t>
+  </si>
+  <si>
+    <t>MSFT UW</t>
+  </si>
+  <si>
+    <t>Microsoft Corporation</t>
+  </si>
+  <si>
+    <t>AMZN UQ</t>
+  </si>
+  <si>
+    <t>Amazon.com Inc.</t>
+  </si>
+  <si>
+    <t>ADBE UQ</t>
+  </si>
+  <si>
+    <t>Adobe Inc.</t>
+  </si>
+  <si>
+    <t>NVDA UQ</t>
+  </si>
+  <si>
+    <t>NVIDIA CORP (USD)</t>
+  </si>
+  <si>
+    <t>NASDAQ Global Market</t>
+  </si>
+  <si>
+    <t>Taiwan Semiconductor SP ADR(USD)</t>
+  </si>
+  <si>
+    <t>NYSE Market (DE), Inc.</t>
+  </si>
+  <si>
+    <t>NOW UN</t>
+  </si>
+  <si>
+    <t>ServiceNow, Inc.</t>
+  </si>
+  <si>
+    <t>New York Stock Exchange</t>
+  </si>
+  <si>
+    <t>CRM UN</t>
+  </si>
+  <si>
+    <t>Salesforce, Inc.</t>
+  </si>
+  <si>
+    <t>MGM UN</t>
+  </si>
+  <si>
+    <t>MGM Resorts International</t>
+  </si>
+  <si>
+    <t>SMCI UQ</t>
+  </si>
+  <si>
+    <t>Super Micro Computer, Inc.</t>
+  </si>
+  <si>
+    <t>AAPL UQ</t>
+  </si>
+  <si>
+    <t>Apple Inc.</t>
+  </si>
+  <si>
+    <t>TSLA UQ</t>
+  </si>
+  <si>
+    <t>Tesla Inc.(USD)</t>
+  </si>
+  <si>
+    <t>INTC UQ</t>
+  </si>
+  <si>
+    <t>Intel Corporation</t>
+  </si>
+  <si>
+    <t>AVGO UQ</t>
+  </si>
+  <si>
+    <t>Broadcom Inc.</t>
+  </si>
+  <si>
+    <t>Qualcomm Incorporated</t>
+  </si>
+  <si>
+    <t>PANW UQ</t>
+  </si>
+  <si>
+    <t>Advanced Micro Devices (USD)</t>
+  </si>
+  <si>
+    <t>AMD UQ</t>
+  </si>
+  <si>
+    <t>Palo Alto Networks Inc.</t>
+  </si>
+  <si>
+    <t>DVN UN</t>
+  </si>
+  <si>
+    <t>Devon Energy Corporation</t>
+  </si>
+  <si>
+    <t>OXY UN</t>
+  </si>
+  <si>
+    <t>Occidental Petroleum Corporation</t>
+  </si>
+  <si>
+    <t>XOM UN</t>
+  </si>
+  <si>
+    <t>Exxon Mobil Corporation</t>
+  </si>
+  <si>
+    <t>FANG UQ</t>
+  </si>
+  <si>
+    <t>Diamondback Energy Inc,</t>
+  </si>
+  <si>
+    <t>MRO UN</t>
+  </si>
+  <si>
+    <t>Marathon Oil Corp</t>
+  </si>
+  <si>
+    <t>SLB UN</t>
+  </si>
+  <si>
+    <t>Schlumberger N.V (Schlumberger Limited)</t>
+  </si>
+  <si>
+    <t>HAL UN</t>
+  </si>
+  <si>
+    <t>Halliburton Company</t>
+  </si>
+  <si>
+    <t>MRVL UQ</t>
+  </si>
+  <si>
+    <t>Marvell Technology, Inc.</t>
+  </si>
+  <si>
+    <t>EOG UN</t>
+  </si>
+  <si>
+    <t>EOG Resources Inc.</t>
+  </si>
+  <si>
+    <t>DDOG UQ</t>
+  </si>
+  <si>
+    <t>Datadog Inc - Class A (USD)</t>
+  </si>
+  <si>
+    <t>NFLX UW</t>
+  </si>
+  <si>
+    <t>Netflix Inc.(USD)</t>
+  </si>
+  <si>
+    <t>GOOGL UW</t>
+  </si>
+  <si>
+    <t>Alphabet Inc -Class A (USD)</t>
+  </si>
+  <si>
+    <t>PARA UQ</t>
+  </si>
+  <si>
+    <t>Paramount Global Class B (USD)</t>
+  </si>
+  <si>
+    <t>WBD UQ</t>
+  </si>
+  <si>
+    <t>Warner Bros Discovery Inc.(USD)</t>
+  </si>
+  <si>
+    <t>LVS UN</t>
+  </si>
+  <si>
+    <t>Las Vegas Sands Corp(USD)</t>
+  </si>
+  <si>
+    <t>WYNN UQ</t>
+  </si>
+  <si>
+    <t>Wynn Resorts LTD(USD)</t>
+  </si>
+  <si>
+    <t>ABBN SE</t>
+  </si>
+  <si>
+    <t>ABB Ltd</t>
+  </si>
+  <si>
+    <t>SIX Swiss Exchange AG</t>
+  </si>
+  <si>
+    <t>GIVN SE</t>
+  </si>
+  <si>
+    <t>Givaudan SA</t>
+  </si>
+  <si>
+    <t>NOVN SE</t>
+  </si>
+  <si>
+    <t>Novartis AG</t>
+  </si>
+  <si>
+    <t>AMAT UQ</t>
+  </si>
+  <si>
+    <t>APPLIED MATERIALS INC (USD)</t>
+  </si>
+  <si>
+    <t>GLD UP</t>
+  </si>
+  <si>
+    <t>SPDR GOLD SHARES (USD)</t>
+  </si>
+  <si>
+    <t>PACIFIC STOCK EXCHANGE INC</t>
+  </si>
+  <si>
+    <t>GDX UP</t>
+  </si>
+  <si>
+    <t>VANECK GOLD MINERS ETF (USD)</t>
+  </si>
+  <si>
+    <t>META UQ</t>
+  </si>
+  <si>
+    <t>META PLATFORMS INC-CLASS A (USD)</t>
+  </si>
+  <si>
+    <t>UBER UN</t>
+  </si>
+  <si>
+    <t>UBER TECHNOLOGIES INC (USD)</t>
+  </si>
+  <si>
+    <t>NYSE MARKET (DE), INC</t>
+  </si>
+  <si>
+    <t>VLO UN</t>
+  </si>
+  <si>
+    <t>VALERO ENERGY CORP (USD)</t>
+  </si>
+  <si>
+    <t>BAC UN</t>
+  </si>
+  <si>
+    <t>BANK OF AMERICA CORP (USD)</t>
+  </si>
+  <si>
+    <t>WFC UN</t>
+  </si>
+  <si>
+    <t>WELLS FARGO &amp; CO (USD)</t>
+  </si>
+  <si>
+    <t>C UN</t>
+  </si>
+  <si>
+    <t>CITIGROUP INC (USD)</t>
+  </si>
+  <si>
+    <t>TSLA UW</t>
+  </si>
+  <si>
+    <t>MSFT UQ</t>
+  </si>
+  <si>
+    <t>DIS UN</t>
+  </si>
+  <si>
+    <t>The Walt Disney Company</t>
+  </si>
+  <si>
+    <t>MPACT SP</t>
+  </si>
+  <si>
+    <t>MapleTree Pan Asia Com Trust</t>
+  </si>
+  <si>
+    <t>Singapore Exchange Limited</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>FLT SP</t>
+  </si>
+  <si>
+    <t>Frasers Logistics &amp; Commerci</t>
+  </si>
+  <si>
+    <t>1772 HK</t>
+  </si>
+  <si>
+    <t>Ganfeng Lithium Co., Ltd.</t>
+  </si>
+  <si>
+    <t>The Stock Exchange of Hong Kong Ltd</t>
+  </si>
+  <si>
+    <t>HKD</t>
+  </si>
+  <si>
+    <t>291 HK</t>
+  </si>
+  <si>
+    <t>China Resources Beer Holdings</t>
+  </si>
+  <si>
+    <t>PDD UQ</t>
+  </si>
+  <si>
+    <t>PDD Holdings Inc.</t>
+  </si>
+  <si>
+    <t>SOXX UQ</t>
+  </si>
+  <si>
+    <t>iShares Semiconductor ETF</t>
+  </si>
+  <si>
+    <t>9988 HK</t>
+  </si>
+  <si>
+    <t>ALIBABA GROUP HOLDING LTD (HKD)</t>
+  </si>
+  <si>
+    <t>9901 HK</t>
+  </si>
+  <si>
+    <t>NEW ORIENTAL EDUCATION &amp; TEC (HKD)</t>
+  </si>
+  <si>
+    <t>(i)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Initial Share Price</t>
+  </si>
+  <si>
+    <t>Strike Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +572,20 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -343,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -393,6 +790,22 @@
     <xf numFmtId="10" fontId="5" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,6 +821,60 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Input"/>
+      <sheetName val="Temp Paths"/>
+      <sheetName val="CONFIG"/>
+      <sheetName val="Main"/>
+      <sheetName val="Client Changes DATABASE"/>
+      <sheetName val="BBG CODE"/>
+      <sheetName val="Capped Booster DATABASE"/>
+      <sheetName val="BEN DATABASE"/>
+      <sheetName val="DCN DATABASE"/>
+      <sheetName val="BEN Payoff"/>
+      <sheetName val="DCN Payoff"/>
+      <sheetName val="Client Based Changes"/>
+      <sheetName val="Product Details"/>
+      <sheetName val="Payoff Table"/>
+      <sheetName val="Share Basket DATABASE"/>
+      <sheetName val="Share Basket"/>
+      <sheetName val="Observation Date"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v>No EKI</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -676,7 +1143,7 @@
   <dimension ref="B3:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,14 +1213,12 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="5"/>
       <c r="H5" s="4">
         <v>85</v>
@@ -799,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FCCAF5-58C3-4D44-9C49-A1FEBE5D251F}">
   <dimension ref="B3:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -835,14 +1300,14 @@
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="str">
         <f ca="1">TEXT(TODAY(),"dd mmmm yyyy")</f>
-        <v>06 March 2025</v>
+        <v>10 March 2025</v>
       </c>
       <c r="C5" s="4" t="str">
         <f ca="1">B5</f>
-        <v>06 March 2025</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>10 March 2025</v>
+      </c>
+      <c r="D5" s="17">
+        <v>600000</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>9</v>
@@ -867,7 +1332,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,7 +1341,7 @@
     <col min="7" max="10" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
@@ -1530,4 +1995,980 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85621591-9667-4D08-91AC-71BDD3D083C0}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="20" t="str">
+        <f>IF('[1]Product Details'!D1="No EKI","Coupon Barrier Price","Knock-in Price")</f>
+        <v>Coupon Barrier Price</v>
+      </c>
+      <c r="I1" s="20" t="str">
+        <f>IF('[1]Product Details'!D1="No EKI","","Coupon Barrier Price")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="str">
+        <f>VLOOKUP(C2,'BBG CODES'!A:D,2,FALSE)</f>
+        <v>Alphabet Inc.</v>
+      </c>
+      <c r="C2" s="22" t="str">
+        <f>Main!D5</f>
+        <v>GOOGL UQ</v>
+      </c>
+      <c r="D2" s="22" t="str">
+        <f>VLOOKUP(C2,'BBG CODES'!A:D,3,FALSE)</f>
+        <v>NASDAQ Global Select Market</v>
+      </c>
+      <c r="E2" s="22" t="str">
+        <f>VLOOKUP(C2,'BBG CODES'!A:E,4,FALSE)</f>
+        <v>USD</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21">
+        <f>IF(B3="","",A2+1)</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C3,'BBG CODES'!A:D,2,FALSE),"")</f>
+        <v>Amazon.com Inc.</v>
+      </c>
+      <c r="C3" s="22" t="str">
+        <f>Main!E5</f>
+        <v>AMZN UQ</v>
+      </c>
+      <c r="D3" s="22" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C3,'BBG CODES'!A:D,3,FALSE),"")</f>
+        <v>NASDAQ Global Select Market</v>
+      </c>
+      <c r="E3" s="22" t="str">
+        <f>VLOOKUP(C3,'BBG CODES'!A:E,4,FALSE)</f>
+        <v>USD</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="str">
+        <f>IF(B4="","",A3+1)</f>
+        <v/>
+      </c>
+      <c r="B4" s="21" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C4,'BBG CODES'!A:D,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="C4" s="22" t="str">
+        <f>IF(Main!F5="","",Main!F5)</f>
+        <v/>
+      </c>
+      <c r="D4" s="22" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C4,'BBG CODES'!A:D,3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="E4" s="22" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C4,'BBG CODES'!A:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="str">
+        <f>IF(B5="","",A4+1)</f>
+        <v/>
+      </c>
+      <c r="B5" s="21" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C5,'BBG CODES'!A:D,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="C5" s="22" t="str">
+        <f>IF(Main!G5="","",Main!G5)</f>
+        <v/>
+      </c>
+      <c r="D5" s="22" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C5,'BBG CODES'!A:D,3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="E5" s="22" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C5,'BBG CODES'!A:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8423893D-5F5D-4D23-A981-AE5FA9F90797}">
+  <dimension ref="A1:D58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>137</v>
+      </c>
+      <c r="B49" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" t="s">
+        <v>141</v>
+      </c>
+      <c r="D52" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54" t="s">
+        <v>150</v>
+      </c>
+      <c r="C54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" t="s">
+        <v>154</v>
+      </c>
+      <c r="C56" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" t="s">
+        <v>147</v>
+      </c>
+      <c r="D57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" t="s">
+        <v>147</v>
+      </c>
+      <c r="D58" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>